<commit_message>
worked on excel function
</commit_message>
<xml_diff>
--- a/MyfirstMavenProjectIT/Data/MercuryTourFlights.xlsx
+++ b/MyfirstMavenProjectIT/Data/MercuryTourFlights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junaid\git\ITHEALTH.RepoCSVmongoTables\MyfirstMavenProjectIT\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DF84D5-74F8-43A7-82BE-F8D36A87246B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BE569C-D724-48BB-8EF1-7C25762D2A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3C5AB9A-E5DE-49D2-B132-75393F7B4069}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Arriving in</t>
   </si>
@@ -59,24 +59,6 @@
   </si>
   <si>
     <t>August</t>
-  </si>
-  <si>
-    <t>Departing From</t>
-  </si>
-  <si>
-    <t>Departing day</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Departing  Month</t>
-  </si>
-  <si>
-    <t>Returning  month</t>
-  </si>
-  <si>
-    <t>Returning Day</t>
-  </si>
-  <si>
-    <t>Returning from</t>
   </si>
 </sst>
 </file>
@@ -112,11 +94,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,84 +414,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A448A81D-EBE6-4FFD-BF34-EF9E3774D38A}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.21875" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2">
         <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3">
+      <c r="F2" s="2">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
commit from my side
</commit_message>
<xml_diff>
--- a/MyfirstMavenProjectIT/Data/MercuryTourFlights.xlsx
+++ b/MyfirstMavenProjectIT/Data/MercuryTourFlights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junaid\git\ITHEALTH.RepoCSVmongoTables\MyfirstMavenProjectIT\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\ITHEALTH.RepoCSVmongoTables\MyfirstMavenProjectIT\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283A72B7-58C8-4105-AB1B-11231E5EB886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311F07AC-59EE-478D-8BCB-8A896642C692}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3C5AB9A-E5DE-49D2-B132-75393F7B4069}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3C5AB9A-E5DE-49D2-B132-75393F7B4069}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Arriving in</t>
   </si>
@@ -59,6 +59,30 @@
   </si>
   <si>
     <t>August</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>fromM</t>
+  </si>
+  <si>
+    <t>fromD</t>
+  </si>
+  <si>
+    <t>return</t>
+  </si>
+  <si>
+    <t>returnM</t>
+  </si>
+  <si>
+    <t>returnD</t>
   </si>
 </sst>
 </file>
@@ -414,63 +438,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A448A81D-EBE6-4FFD-BF34-EF9E3774D38A}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C2" s="2">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F2" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -488,6 +512,26 @@
       </c>
       <c r="F3" s="2">
         <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -504,9 +548,9 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +561,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -528,7 +572,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>

</xml_diff>